<commit_message>
Further attempts on the synthetic control and aDID
</commit_message>
<xml_diff>
--- a/Replication files/Decile Analysis/Coefficient Tables/exported_tables.xlsx
+++ b/Replication files/Decile Analysis/Coefficient Tables/exported_tables.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="158">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="117">
   <si>
     <t xml:space="preserve">tau</t>
   </si>
@@ -113,7 +113,7 @@
     <t xml:space="preserve">0.0001334</t>
   </si>
   <si>
-    <t xml:space="preserve">1.192***</t>
+    <t xml:space="preserve">1.192**</t>
   </si>
   <si>
     <t xml:space="preserve">2.687***</t>
@@ -245,7 +245,7 @@
     <t xml:space="preserve">ln_battle_fatalities</t>
   </si>
   <si>
-    <t xml:space="preserve">-0.1584*</t>
+    <t xml:space="preserve">-0.1584**</t>
   </si>
   <si>
     <t xml:space="preserve">log_GDP_r</t>
@@ -305,7 +305,7 @@
     <t xml:space="preserve">-1.344***</t>
   </si>
   <si>
-    <t xml:space="preserve">0.0003315*</t>
+    <t xml:space="preserve">0.0003315.</t>
   </si>
   <si>
     <t xml:space="preserve">-0.143***</t>
@@ -353,7 +353,7 @@
     <t xml:space="preserve">15.94***</t>
   </si>
   <si>
-    <t xml:space="preserve">-0.002022</t>
+    <t xml:space="preserve">-0.002022.</t>
   </si>
   <si>
     <t xml:space="preserve">-0.3374***</t>
@@ -363,129 +363,6 @@
   </si>
   <si>
     <t xml:space="preserve">passengers.in.change.pct + ln_battle_fatalities + log_GDP_r</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-44.65***</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.0001585</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.04635*</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2.492***</t>
-  </si>
-  <si>
-    <t xml:space="preserve">4.328***</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-1.268**</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1.438**</t>
-  </si>
-  <si>
-    <t xml:space="preserve">9.489***</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-1.876***</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3.313***</t>
-  </si>
-  <si>
-    <t xml:space="preserve">6.792***</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.3849</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-2.293.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1.9***</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.5529</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-2.401**</t>
-  </si>
-  <si>
-    <t xml:space="preserve">7.602***</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.3356</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1.389*</t>
-  </si>
-  <si>
-    <t xml:space="preserve">7.307***</t>
-  </si>
-  <si>
-    <t xml:space="preserve">passengers.in.change.pct + ln_battle_fatalities + log_GDP_r + factor(Country.Name)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">17.3***</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.0001517</t>
-  </si>
-  <si>
-    <t xml:space="preserve">18.48***</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.0005627</t>
-  </si>
-  <si>
-    <t xml:space="preserve">19.32***</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.0002096</t>
-  </si>
-  <si>
-    <t xml:space="preserve">19.91***</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.0002852</t>
-  </si>
-  <si>
-    <t xml:space="preserve">20.47***</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-2.466e-05</t>
-  </si>
-  <si>
-    <t xml:space="preserve">21.05***</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-1.647e-05</t>
-  </si>
-  <si>
-    <t xml:space="preserve">21.72***</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.0001547</t>
-  </si>
-  <si>
-    <t xml:space="preserve">22.69***</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.0007065**</t>
-  </si>
-  <si>
-    <t xml:space="preserve">23.87***</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.0009211**</t>
-  </si>
-  <si>
-    <t xml:space="preserve">27.33***</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.002846</t>
   </si>
 </sst>
 </file>
@@ -854,24 +731,6 @@
       <c r="L1" t="s">
         <v>2</v>
       </c>
-      <c r="M1" t="s">
-        <v>0</v>
-      </c>
-      <c r="N1" t="s">
-        <v>1</v>
-      </c>
-      <c r="O1" t="s">
-        <v>2</v>
-      </c>
-      <c r="P1" t="s">
-        <v>0</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>1</v>
-      </c>
-      <c r="R1" t="s">
-        <v>2</v>
-      </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
@@ -910,24 +769,6 @@
       <c r="L2" t="s">
         <v>73</v>
       </c>
-      <c r="M2" t="n">
-        <v>0.1</v>
-      </c>
-      <c r="N2" t="s">
-        <v>3</v>
-      </c>
-      <c r="O2" t="s">
-        <v>117</v>
-      </c>
-      <c r="P2" t="n">
-        <v>0.1</v>
-      </c>
-      <c r="Q2" t="s">
-        <v>3</v>
-      </c>
-      <c r="R2" t="s">
-        <v>138</v>
-      </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
@@ -966,24 +807,6 @@
       <c r="L3" t="s">
         <v>75</v>
       </c>
-      <c r="M3" t="n">
-        <v>0.1</v>
-      </c>
-      <c r="N3" t="s">
-        <v>74</v>
-      </c>
-      <c r="O3" t="s">
-        <v>118</v>
-      </c>
-      <c r="P3" t="n">
-        <v>0.1</v>
-      </c>
-      <c r="Q3" t="s">
-        <v>74</v>
-      </c>
-      <c r="R3" t="s">
-        <v>139</v>
-      </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
@@ -1022,24 +845,6 @@
       <c r="L4" t="s">
         <v>77</v>
       </c>
-      <c r="M4" t="n">
-        <v>0.2</v>
-      </c>
-      <c r="N4" t="s">
-        <v>3</v>
-      </c>
-      <c r="O4" t="s">
-        <v>119</v>
-      </c>
-      <c r="P4" t="n">
-        <v>0.2</v>
-      </c>
-      <c r="Q4" t="s">
-        <v>3</v>
-      </c>
-      <c r="R4" t="s">
-        <v>140</v>
-      </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
@@ -1078,24 +883,6 @@
       <c r="L5" t="s">
         <v>79</v>
       </c>
-      <c r="M5" t="n">
-        <v>0.2</v>
-      </c>
-      <c r="N5" t="s">
-        <v>74</v>
-      </c>
-      <c r="O5" t="s">
-        <v>120</v>
-      </c>
-      <c r="P5" t="n">
-        <v>0.2</v>
-      </c>
-      <c r="Q5" t="s">
-        <v>74</v>
-      </c>
-      <c r="R5" t="s">
-        <v>141</v>
-      </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
@@ -1134,24 +921,6 @@
       <c r="L6" t="s">
         <v>80</v>
       </c>
-      <c r="M6" t="n">
-        <v>0.3</v>
-      </c>
-      <c r="N6" t="s">
-        <v>3</v>
-      </c>
-      <c r="O6" t="s">
-        <v>121</v>
-      </c>
-      <c r="P6" t="n">
-        <v>0.3</v>
-      </c>
-      <c r="Q6" t="s">
-        <v>3</v>
-      </c>
-      <c r="R6" t="s">
-        <v>142</v>
-      </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
@@ -1190,24 +959,6 @@
       <c r="L7" t="s">
         <v>81</v>
       </c>
-      <c r="M7" t="n">
-        <v>0.3</v>
-      </c>
-      <c r="N7" t="s">
-        <v>74</v>
-      </c>
-      <c r="O7" t="s">
-        <v>122</v>
-      </c>
-      <c r="P7" t="n">
-        <v>0.3</v>
-      </c>
-      <c r="Q7" t="s">
-        <v>74</v>
-      </c>
-      <c r="R7" t="s">
-        <v>143</v>
-      </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
@@ -1246,24 +997,6 @@
       <c r="L8" t="s">
         <v>82</v>
       </c>
-      <c r="M8" t="n">
-        <v>0.4</v>
-      </c>
-      <c r="N8" t="s">
-        <v>3</v>
-      </c>
-      <c r="O8" t="s">
-        <v>123</v>
-      </c>
-      <c r="P8" t="n">
-        <v>0.4</v>
-      </c>
-      <c r="Q8" t="s">
-        <v>3</v>
-      </c>
-      <c r="R8" t="s">
-        <v>144</v>
-      </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
@@ -1302,24 +1035,6 @@
       <c r="L9" t="s">
         <v>83</v>
       </c>
-      <c r="M9" t="n">
-        <v>0.4</v>
-      </c>
-      <c r="N9" t="s">
-        <v>74</v>
-      </c>
-      <c r="O9" t="s">
-        <v>124</v>
-      </c>
-      <c r="P9" t="n">
-        <v>0.4</v>
-      </c>
-      <c r="Q9" t="s">
-        <v>74</v>
-      </c>
-      <c r="R9" t="s">
-        <v>145</v>
-      </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
@@ -1358,24 +1073,6 @@
       <c r="L10" t="s">
         <v>84</v>
       </c>
-      <c r="M10" t="n">
-        <v>0.5</v>
-      </c>
-      <c r="N10" t="s">
-        <v>3</v>
-      </c>
-      <c r="O10" t="s">
-        <v>125</v>
-      </c>
-      <c r="P10" t="n">
-        <v>0.5</v>
-      </c>
-      <c r="Q10" t="s">
-        <v>3</v>
-      </c>
-      <c r="R10" t="s">
-        <v>146</v>
-      </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
@@ -1414,24 +1111,6 @@
       <c r="L11" t="s">
         <v>85</v>
       </c>
-      <c r="M11" t="n">
-        <v>0.5</v>
-      </c>
-      <c r="N11" t="s">
-        <v>74</v>
-      </c>
-      <c r="O11" t="s">
-        <v>126</v>
-      </c>
-      <c r="P11" t="n">
-        <v>0.5</v>
-      </c>
-      <c r="Q11" t="s">
-        <v>74</v>
-      </c>
-      <c r="R11" t="s">
-        <v>147</v>
-      </c>
     </row>
     <row r="12">
       <c r="A12" t="n">
@@ -1470,24 +1149,6 @@
       <c r="L12" t="s">
         <v>86</v>
       </c>
-      <c r="M12" t="n">
-        <v>0.6</v>
-      </c>
-      <c r="N12" t="s">
-        <v>3</v>
-      </c>
-      <c r="O12" t="s">
-        <v>127</v>
-      </c>
-      <c r="P12" t="n">
-        <v>0.6</v>
-      </c>
-      <c r="Q12" t="s">
-        <v>3</v>
-      </c>
-      <c r="R12" t="s">
-        <v>148</v>
-      </c>
     </row>
     <row r="13">
       <c r="A13" t="n">
@@ -1526,24 +1187,6 @@
       <c r="L13" t="s">
         <v>87</v>
       </c>
-      <c r="M13" t="n">
-        <v>0.6</v>
-      </c>
-      <c r="N13" t="s">
-        <v>74</v>
-      </c>
-      <c r="O13" t="s">
-        <v>128</v>
-      </c>
-      <c r="P13" t="n">
-        <v>0.6</v>
-      </c>
-      <c r="Q13" t="s">
-        <v>74</v>
-      </c>
-      <c r="R13" t="s">
-        <v>149</v>
-      </c>
     </row>
     <row r="14">
       <c r="A14" t="n">
@@ -1582,24 +1225,6 @@
       <c r="L14" t="s">
         <v>88</v>
       </c>
-      <c r="M14" t="n">
-        <v>0.7</v>
-      </c>
-      <c r="N14" t="s">
-        <v>3</v>
-      </c>
-      <c r="O14" t="s">
-        <v>129</v>
-      </c>
-      <c r="P14" t="n">
-        <v>0.7</v>
-      </c>
-      <c r="Q14" t="s">
-        <v>3</v>
-      </c>
-      <c r="R14" t="s">
-        <v>150</v>
-      </c>
     </row>
     <row r="15">
       <c r="A15" t="n">
@@ -1638,24 +1263,6 @@
       <c r="L15" t="s">
         <v>89</v>
       </c>
-      <c r="M15" t="n">
-        <v>0.7</v>
-      </c>
-      <c r="N15" t="s">
-        <v>74</v>
-      </c>
-      <c r="O15" t="s">
-        <v>130</v>
-      </c>
-      <c r="P15" t="n">
-        <v>0.7</v>
-      </c>
-      <c r="Q15" t="s">
-        <v>74</v>
-      </c>
-      <c r="R15" t="s">
-        <v>151</v>
-      </c>
     </row>
     <row r="16">
       <c r="A16" t="n">
@@ -1694,24 +1301,6 @@
       <c r="L16" t="s">
         <v>90</v>
       </c>
-      <c r="M16" t="n">
-        <v>0.8</v>
-      </c>
-      <c r="N16" t="s">
-        <v>3</v>
-      </c>
-      <c r="O16" t="s">
-        <v>131</v>
-      </c>
-      <c r="P16" t="n">
-        <v>0.8</v>
-      </c>
-      <c r="Q16" t="s">
-        <v>3</v>
-      </c>
-      <c r="R16" t="s">
-        <v>152</v>
-      </c>
     </row>
     <row r="17">
       <c r="A17" t="n">
@@ -1750,24 +1339,6 @@
       <c r="L17" t="s">
         <v>91</v>
       </c>
-      <c r="M17" t="n">
-        <v>0.8</v>
-      </c>
-      <c r="N17" t="s">
-        <v>74</v>
-      </c>
-      <c r="O17" t="s">
-        <v>132</v>
-      </c>
-      <c r="P17" t="n">
-        <v>0.8</v>
-      </c>
-      <c r="Q17" t="s">
-        <v>74</v>
-      </c>
-      <c r="R17" t="s">
-        <v>153</v>
-      </c>
     </row>
     <row r="18">
       <c r="A18" t="n">
@@ -1806,24 +1377,6 @@
       <c r="L18" t="s">
         <v>92</v>
       </c>
-      <c r="M18" t="n">
-        <v>0.9</v>
-      </c>
-      <c r="N18" t="s">
-        <v>3</v>
-      </c>
-      <c r="O18" t="s">
-        <v>133</v>
-      </c>
-      <c r="P18" t="n">
-        <v>0.9</v>
-      </c>
-      <c r="Q18" t="s">
-        <v>3</v>
-      </c>
-      <c r="R18" t="s">
-        <v>154</v>
-      </c>
     </row>
     <row r="19">
       <c r="A19" t="n">
@@ -1862,24 +1415,6 @@
       <c r="L19" t="s">
         <v>93</v>
       </c>
-      <c r="M19" t="n">
-        <v>0.9</v>
-      </c>
-      <c r="N19" t="s">
-        <v>74</v>
-      </c>
-      <c r="O19" t="s">
-        <v>134</v>
-      </c>
-      <c r="P19" t="n">
-        <v>0.9</v>
-      </c>
-      <c r="Q19" t="s">
-        <v>74</v>
-      </c>
-      <c r="R19" t="s">
-        <v>155</v>
-      </c>
     </row>
     <row r="20">
       <c r="A20" t="n">
@@ -1918,24 +1453,6 @@
       <c r="L20" t="s">
         <v>94</v>
       </c>
-      <c r="M20" t="n">
-        <v>1</v>
-      </c>
-      <c r="N20" t="s">
-        <v>3</v>
-      </c>
-      <c r="O20" t="s">
-        <v>135</v>
-      </c>
-      <c r="P20" t="n">
-        <v>1</v>
-      </c>
-      <c r="Q20" t="s">
-        <v>3</v>
-      </c>
-      <c r="R20" t="s">
-        <v>156</v>
-      </c>
     </row>
     <row r="21">
       <c r="A21" t="n">
@@ -1973,24 +1490,6 @@
       </c>
       <c r="L21" t="s">
         <v>95</v>
-      </c>
-      <c r="M21" t="n">
-        <v>1</v>
-      </c>
-      <c r="N21" t="s">
-        <v>74</v>
-      </c>
-      <c r="O21" t="s">
-        <v>136</v>
-      </c>
-      <c r="P21" t="n">
-        <v>1</v>
-      </c>
-      <c r="Q21" t="s">
-        <v>74</v>
-      </c>
-      <c r="R21" t="s">
-        <v>157</v>
       </c>
     </row>
     <row r="22">
@@ -2012,12 +1511,6 @@
       <c r="L22" t="s">
         <v>96</v>
       </c>
-      <c r="M22"/>
-      <c r="N22"/>
-      <c r="O22"/>
-      <c r="P22"/>
-      <c r="Q22"/>
-      <c r="R22"/>
     </row>
     <row r="23">
       <c r="A23"/>
@@ -2050,20 +1543,6 @@
       <c r="L23" t="s">
         <v>97</v>
       </c>
-      <c r="M23"/>
-      <c r="N23" t="s">
-        <v>25</v>
-      </c>
-      <c r="O23" t="s">
-        <v>26</v>
-      </c>
-      <c r="P23"/>
-      <c r="Q23" t="s">
-        <v>25</v>
-      </c>
-      <c r="R23" t="s">
-        <v>26</v>
-      </c>
     </row>
     <row r="24">
       <c r="A24"/>
@@ -2096,20 +1575,6 @@
       <c r="L24" t="s">
         <v>98</v>
       </c>
-      <c r="M24"/>
-      <c r="N24" t="s">
-        <v>25</v>
-      </c>
-      <c r="O24" t="s">
-        <v>27</v>
-      </c>
-      <c r="P24"/>
-      <c r="Q24" t="s">
-        <v>25</v>
-      </c>
-      <c r="R24" t="s">
-        <v>27</v>
-      </c>
     </row>
     <row r="25">
       <c r="A25"/>
@@ -2142,20 +1607,6 @@
       <c r="L25" t="s">
         <v>99</v>
       </c>
-      <c r="M25"/>
-      <c r="N25" t="s">
-        <v>25</v>
-      </c>
-      <c r="O25" t="s">
-        <v>137</v>
-      </c>
-      <c r="P25"/>
-      <c r="Q25" t="s">
-        <v>25</v>
-      </c>
-      <c r="R25" t="s">
-        <v>74</v>
-      </c>
     </row>
     <row r="26">
       <c r="A26"/>
@@ -2187,20 +1638,6 @@
       </c>
       <c r="L26" t="s">
         <v>100</v>
-      </c>
-      <c r="M26"/>
-      <c r="N26" t="s">
-        <v>28</v>
-      </c>
-      <c r="O26" t="s">
-        <v>29</v>
-      </c>
-      <c r="P26"/>
-      <c r="Q26" t="s">
-        <v>28</v>
-      </c>
-      <c r="R26" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="27">

</xml_diff>